<commit_message>
- start modeling WorkEstimateExcelDTO - implementing xlsx writer - in progress - update model :) -
</commit_message>
<xml_diff>
--- a/src/main/resources/xls/Work-Estimate.xlsx
+++ b/src/main/resources/xls/Work-Estimate.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\$SDA\IntelllyJ_projects\13.projektGrupowy\ContainerApp\src\main\resources\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6141937E-CD64-4149-B158-5A5B58782524}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="360" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve"> REPAIR ESTIMATE</t>
   </si>
@@ -88,19 +102,7 @@
     <t>EUR</t>
   </si>
   <si>
-    <t>Terminal  Poznań</t>
-  </si>
-  <si>
-    <t>45'HW</t>
-  </si>
-  <si>
     <t>Repair handling</t>
-  </si>
-  <si>
-    <t>NNNU</t>
-  </si>
-  <si>
-    <t>123456</t>
   </si>
   <si>
     <t xml:space="preserve">Gestia Armatora </t>
@@ -109,13 +111,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;     &quot;@"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
     <numFmt numFmtId="166" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="167" formatCode="&quot;   &quot;@"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1414,12 +1416,12 @@
     <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="58" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1518,29 +1520,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1554,20 +1538,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1575,65 +1627,35 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1655,12 +1677,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1719,133 +1735,119 @@
     <xf numFmtId="167" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="20% - akcent 1" xfId="18" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 2" xfId="22" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 3" xfId="26" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 4" xfId="30" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 5" xfId="34" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - akcent 6" xfId="38" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 1" xfId="19" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 2" xfId="23" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 3" xfId="27" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 4" xfId="31" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 5" xfId="35" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - akcent 6" xfId="39" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 1" xfId="20" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 2" xfId="24" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 3" xfId="28" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 4" xfId="32" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 5" xfId="36" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - akcent 6" xfId="40" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 3" xfId="26" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 4" xfId="30" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 5" xfId="34" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 6" xfId="38" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 3" xfId="27" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 4" xfId="31" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 5" xfId="35" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 6" xfId="39" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 1" xfId="20" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 2" xfId="24" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 3" xfId="28" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 4" xfId="32" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 5" xfId="36" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 6" xfId="40" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Akcent 1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Akcent 2" xfId="21" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Akcent 3" xfId="25" builtinId="37" customBuiltin="1"/>
@@ -1854,29 +1856,29 @@
     <cellStyle name="Akcent 6" xfId="37" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Dane wejściowe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Dane wyjściowe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Dobre" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Dziesiętny 2" xfId="45"/>
-    <cellStyle name="Dziesiętny 3" xfId="46"/>
-    <cellStyle name="Dziesiętny 4" xfId="47"/>
-    <cellStyle name="Dziesiętny 5" xfId="48"/>
-    <cellStyle name="Dziesiętny 6" xfId="43"/>
+    <cellStyle name="Dobry" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Dziesiętny 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Dziesiętny 3" xfId="46" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Dziesiętny 4" xfId="47" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Dziesiętny 5" xfId="48" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Dziesiętny 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Komórka połączona" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Komórka zaznaczona" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Nagłówek 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Nagłówek 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Nagłówek 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Nagłówek 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutralne" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutralny" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Normalny 2" xfId="41"/>
+    <cellStyle name="Normalny 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Obliczenia" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
     <cellStyle name="Suma" xfId="16" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Tekst objaśnienia" xfId="15" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Tekst ostrzeżenia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Tytuł 2" xfId="44"/>
-    <cellStyle name="Uwaga 2" xfId="42"/>
-    <cellStyle name="Złe" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Tytuł 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Uwaga 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Zły" xfId="7" builtinId="27" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1884,87 +1886,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Obraz 1" descr="LOGO">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D043F5F-E509-4405-B846-00349796D8AC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="914400" y="638175"/>
-          <a:ext cx="1409700" cy="533400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2010,7 +1936,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2043,9 +1969,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2078,6 +2021,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -2253,166 +2213,152 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:K13"/>
+      <selection activeCell="M7" sqref="M7:N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="2" width="13" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="12"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="12"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="123"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="132" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="53"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="133"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
-      <c r="N4" s="134"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="64"/>
     </row>
-    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="126"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="135"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="137"/>
+    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="56"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="67"/>
     </row>
-    <row r="6" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="129"/>
-      <c r="C6" s="130"/>
-      <c r="D6" s="130"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="70" t="s">
+    <row r="6" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="70" t="s">
+      <c r="I6" s="44"/>
+      <c r="J6" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="114"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="70" t="s">
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="71"/>
+      <c r="N6" s="44"/>
     </row>
-    <row r="7" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="115" t="s">
+    <row r="7" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="118" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="120" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="121"/>
-      <c r="L7" s="122"/>
-      <c r="M7" s="118">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="49"/>
+    </row>
+    <row r="8" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="122" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="124"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="125" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="126"/>
+      <c r="J8" s="127"/>
+      <c r="K8" s="128" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="129"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="37"/>
+    </row>
+    <row r="9" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="119"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="128" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="129"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="130"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="39"/>
     </row>
-    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="58"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="61"/>
-      <c r="M8" s="112"/>
-      <c r="N8" s="113"/>
+    <row r="10" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="132"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="134"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="136"/>
+      <c r="L10" s="137"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
     </row>
-    <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="61"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="48">
-        <v>43850</v>
-      </c>
-      <c r="I9" s="49"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="63"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="45"/>
-    </row>
-    <row r="10" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="64" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66">
-        <v>43860</v>
-      </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="47"/>
-    </row>
-    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2425,14 +2371,14 @@
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="111"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="77"/>
       <c r="L11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2441,303 +2387,300 @@
       </c>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
       <c r="L12" s="33"/>
       <c r="M12" s="10"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="29"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
       <c r="L13" s="30"/>
       <c r="M13" s="11"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="29"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="80"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
       <c r="L14" s="30"/>
       <c r="M14" s="11"/>
       <c r="N14" s="7"/>
       <c r="P14" s="28"/>
     </row>
-    <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
       <c r="L15" s="30"/>
       <c r="M15" s="11"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
       <c r="E16" s="34"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
       <c r="L16" s="35"/>
       <c r="M16" s="18"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
       <c r="E17" s="34"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="88"/>
       <c r="L17" s="35"/>
       <c r="M17" s="18"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
       <c r="E18" s="34"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88"/>
       <c r="L18" s="31"/>
-      <c r="M18" s="18">
-        <v>0</v>
-      </c>
+      <c r="M18" s="18"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
       <c r="E19" s="34"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
       <c r="L19" s="31"/>
       <c r="M19" s="18"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
       <c r="E20" s="34"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
       <c r="L20" s="31"/>
       <c r="M20" s="18"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="83" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="85"/>
+      <c r="F21" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="91"/>
       <c r="L21" s="17">
         <v>0</v>
       </c>
-      <c r="M21" s="18">
-        <v>22</v>
-      </c>
+      <c r="M21" s="18"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="88"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="93"/>
+      <c r="J22" s="93"/>
+      <c r="K22" s="94"/>
       <c r="L22" s="17"/>
       <c r="M22" s="18"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="90"/>
-      <c r="K23" s="90"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
       <c r="L23" s="21"/>
       <c r="M23" s="22"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="2:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="91" t="s">
+      <c r="C24" s="110"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="93" t="s">
+      <c r="G24" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
-      <c r="J24" s="95"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="101"/>
       <c r="K24" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L24" s="52"/>
-      <c r="M24" s="53"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="69"/>
       <c r="N24" s="9"/>
     </row>
-    <row r="25" spans="2:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="97"/>
-      <c r="J25" s="98"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="103"/>
+      <c r="J25" s="104"/>
       <c r="K25" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="52">
+      <c r="L25" s="68">
         <f>L24*F26</f>
         <v>0</v>
       </c>
-      <c r="M25" s="53"/>
+      <c r="M25" s="69"/>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="77" t="s">
+    <row r="26" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="72"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="99">
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="105">
         <v>12</v>
       </c>
-      <c r="G26" s="101" t="s">
+      <c r="G26" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="102"/>
-      <c r="I26" s="102"/>
-      <c r="J26" s="103"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="108"/>
+      <c r="J26" s="109"/>
       <c r="K26" s="26"/>
-      <c r="L26" s="52">
+      <c r="L26" s="68">
         <f>SUM(M12:M23)</f>
-        <v>22</v>
-      </c>
-      <c r="M26" s="53"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="69"/>
       <c r="N26" s="9"/>
     </row>
-    <row r="27" spans="2:14" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="78"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="104" t="s">
+    <row r="27" spans="2:14" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="86"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="106"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="72"/>
       <c r="K27" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="L27" s="107">
+      <c r="L27" s="73">
         <f>L26+L25</f>
-        <v>22</v>
-      </c>
-      <c r="M27" s="108"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="74"/>
       <c r="N27" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="M8:N10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="B4:E6"/>
-    <mergeCell ref="F4:N5"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="F11:K11"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F12:K12"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F6:G10"/>
+    <mergeCell ref="H9:J10"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="C26:E27"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="F14:K14"/>
@@ -2754,25 +2697,23 @@
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="F15:K15"/>
     <mergeCell ref="F16:K16"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F6:G10"/>
-    <mergeCell ref="H9:J10"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="F11:K11"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F12:K12"/>
+    <mergeCell ref="M8:N10"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="B4:E6"/>
+    <mergeCell ref="F4:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup scale="79" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>